<commit_message>
Fixed BOM with feedback from European circuits
</commit_message>
<xml_diff>
--- a/bt_bio_bom.xlsx
+++ b/bt_bio_bom.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="101">
-  <si>
-    <t xml:space="preserve">Attys, v0.98</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="105">
+  <si>
+    <t xml:space="preserve">Attys, v0.98b</t>
   </si>
   <si>
     <t xml:space="preserve">Qty</t>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">Farnell</t>
   </si>
   <si>
+    <t xml:space="preserve">RS</t>
+  </si>
+  <si>
     <t xml:space="preserve">MA03-1</t>
   </si>
   <si>
@@ -178,25 +181,34 @@
     <t xml:space="preserve">ADP121-AUJZ18R7</t>
   </si>
   <si>
+    <t xml:space="preserve">SOT95P280X100-5N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150 mA, Low Quiescent Current, CMOS Linear Regulator</t>
+  </si>
+  <si>
     <t xml:space="preserve">ADP121-AUJZ33R7</t>
   </si>
   <si>
-    <t xml:space="preserve">SOT95P280X100-5N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">150 mA, Low Quiescent Current, CMOS Linear Regulator</t>
-  </si>
-  <si>
     <t xml:space="preserve">U1</t>
   </si>
   <si>
+    <t xml:space="preserve">ADS1292RIPBS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TQFP-32</t>
+  </si>
+  <si>
     <t xml:space="preserve">ADS1292R</t>
   </si>
   <si>
-    <t xml:space="preserve">TQFP-32</t>
+    <t xml:space="preserve">Analogue Front End IC, 2-Channel 24 bit, 8ksps SPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">162-6118</t>
   </si>
   <si>
     <t xml:space="preserve">BLUE</t>
@@ -268,7 +280,7 @@
     <t xml:space="preserve">MINI USB Connector</t>
   </si>
   <si>
-    <t xml:space="preserve">MSP430G2553</t>
+    <t xml:space="preserve">MSP430G2553IPW20R</t>
   </si>
   <si>
     <t xml:space="preserve">TSSOP20</t>
@@ -337,6 +349,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -358,17 +371,20 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -413,7 +429,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -434,6 +450,10 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,13 +471,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="29.08"/>
@@ -477,7 +497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -499,22 +519,25 @@
       <c r="G3" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G4" s="3" t="n">
         <v>3417657</v>
@@ -525,19 +548,19 @@
         <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G5" s="3" t="n">
         <v>1759122</v>
@@ -548,19 +571,19 @@
         <v>1</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>15</v>
       </c>
       <c r="G6" s="3" t="n">
         <v>1759102</v>
@@ -571,19 +594,19 @@
         <v>7</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G7" s="3" t="n">
         <v>1458919</v>
@@ -594,19 +617,19 @@
         <v>3</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G8" s="3" t="n">
         <v>1759408</v>
@@ -617,19 +640,19 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G9" s="3" t="n">
         <v>1469765</v>
@@ -640,19 +663,19 @@
         <v>2</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>28</v>
       </c>
       <c r="G10" s="3" t="n">
         <v>1469801</v>
@@ -663,19 +686,19 @@
         <v>2</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G11" s="3" t="n">
         <v>2320809</v>
@@ -686,19 +709,19 @@
         <v>4</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G12" s="3" t="n">
         <v>1754202</v>
@@ -709,19 +732,19 @@
         <v>4</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G13" s="3" t="n">
         <v>1759062</v>
@@ -732,19 +755,19 @@
         <v>1</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G14" s="4" t="n">
         <v>2215655</v>
@@ -755,16 +778,16 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G15" s="3" t="n">
         <v>1101130</v>
@@ -775,19 +798,19 @@
         <v>4</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G16" s="3" t="n">
         <v>2447393</v>
@@ -798,19 +821,19 @@
         <v>2</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G17" s="3" t="n">
         <v>1022276</v>
@@ -821,7 +844,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>52</v>
@@ -836,50 +859,54 @@
         <v>55</v>
       </c>
       <c r="G18" s="3" t="n">
-        <v>2457162</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4026763</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>53</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>55</v>
       </c>
       <c r="G19" s="3" t="n">
-        <v>2074869</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4026766</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="G20" s="3" t="n">
-        <v>3116601</v>
+        <v>60</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -887,19 +914,19 @@
         <v>1</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="G21" s="3" t="n">
         <v>1716765</v>
@@ -910,22 +937,22 @@
         <v>2</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>60</v>
-      </c>
       <c r="D22" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -933,16 +960,16 @@
         <v>1</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="G23" s="3" t="n">
         <v>3123021</v>
@@ -953,19 +980,19 @@
         <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G24" s="3" t="n">
         <v>2532383</v>
@@ -976,16 +1003,16 @@
         <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="G25" s="3" t="n">
         <v>1675426</v>
@@ -996,19 +1023,19 @@
         <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G26" s="3" t="n">
         <v>2293774</v>
@@ -1019,19 +1046,19 @@
         <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="G27" s="3" t="n">
-        <v>2325745</v>
+        <v>3123284</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1039,19 +1066,19 @@
         <v>1</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="G28" s="3" t="n">
         <v>2099241</v>
@@ -1062,16 +1089,16 @@
         <v>1</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="G29" s="3" t="n">
         <v>3580729</v>
@@ -1082,19 +1109,19 @@
         <v>1</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="G30" s="3" t="n">
         <v>1550095</v>
@@ -1105,19 +1132,19 @@
         <v>6</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G31" s="3" t="n">
         <v>8832463</v>
@@ -1128,22 +1155,22 @@
         <v>1</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>